<commit_message>
fix missing/duplicates in dpv, dpv/legal_basis
See Issue #127

-  dpv_legal_basis: Missing concepts for terms defined in main
   vocabulary e.g. dpv:Context
-  dpv: Resolve multiple contributors in term definition e.g.
   isImplementedByEntity
-  dpv: Resolve multiple creation dates in term definition e.g.
   isImplementedByEntity
</commit_message>
<xml_diff>
--- a/code/vocab_csv/rights.xlsx
+++ b/code/vocab_csv/rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="307">
   <si>
     <t>Term</t>
   </si>
@@ -5794,16 +5794,12 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K4" s="21"/>
       <c r="L4" s="19"/>
       <c r="M4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N4" s="19"/>
       <c r="O4" s="33" t="s">
         <v>22</v>
       </c>
@@ -5844,16 +5840,12 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K5" s="21"/>
       <c r="L5" s="19"/>
       <c r="M5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N5" s="19"/>
       <c r="O5" s="33" t="s">
         <v>22</v>
       </c>
@@ -5894,16 +5886,12 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K6" s="21"/>
       <c r="L6" s="19"/>
       <c r="M6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N6" s="19"/>
       <c r="O6" s="33" t="s">
         <v>22</v>
       </c>
@@ -5942,16 +5930,12 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K7" s="21"/>
       <c r="L7" s="19"/>
       <c r="M7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N7" s="19"/>
       <c r="O7" s="33" t="s">
         <v>22</v>
       </c>
@@ -5992,16 +5976,12 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
-      <c r="K8" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K8" s="21"/>
       <c r="L8" s="19"/>
       <c r="M8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N8" s="19"/>
       <c r="O8" s="33" t="s">
         <v>22</v>
       </c>
@@ -6042,16 +6022,12 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
-      <c r="K9" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K9" s="21"/>
       <c r="L9" s="19"/>
       <c r="M9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N9" s="19"/>
       <c r="O9" s="33" t="s">
         <v>22</v>
       </c>
@@ -6092,16 +6068,12 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
-      <c r="K10" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K10" s="21"/>
       <c r="L10" s="19"/>
       <c r="M10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N10" s="19"/>
       <c r="O10" s="33" t="s">
         <v>22</v>
       </c>
@@ -6142,16 +6114,12 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K11" s="21"/>
       <c r="L11" s="19"/>
       <c r="M11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N11" s="19"/>
       <c r="O11" s="33" t="s">
         <v>22</v>
       </c>
@@ -6192,16 +6160,12 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K12" s="21"/>
       <c r="L12" s="19"/>
       <c r="M12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N12" s="19"/>
       <c r="O12" s="33" t="s">
         <v>22</v>
       </c>
@@ -6238,16 +6202,12 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K13" s="21"/>
       <c r="L13" s="19"/>
       <c r="M13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N13" s="19"/>
       <c r="O13" s="33" t="s">
         <v>22</v>
       </c>
@@ -6284,16 +6244,12 @@
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
-      <c r="K14" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K14" s="21"/>
       <c r="L14" s="19"/>
       <c r="M14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N14" s="19"/>
       <c r="O14" s="33" t="s">
         <v>22</v>
       </c>
@@ -6330,16 +6286,12 @@
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
-      <c r="K15" s="21">
-        <v>44867.0</v>
-      </c>
+      <c r="K15" s="21"/>
       <c r="L15" s="19"/>
       <c r="M15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="N15" s="19"/>
       <c r="O15" s="33" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
adds EU NIS2 & RIGHTS documentation; fixes rights
- adds documentation for EU NIS2 (diagrams missing) with note that this
  is a draft vocab
- adds documentation for EU RIGHTS (diagrams missing) with note that this
  is a draft vocab
- fixed issue with EU RIGHTS cocepts where each concept was defined as
  as being narrower than top-concept instead of having a clear hierarchy
</commit_message>
<xml_diff>
--- a/code/vocab_csv/rights.xlsx
+++ b/code/vocab_csv/rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="305">
   <si>
     <t>Term</t>
   </si>
@@ -343,12 +343,6 @@
   </si>
   <si>
     <t>Specfiying the temporal validity of an activity associated with Right Exercise. For example, limits on duration for providing or accessing provided information</t>
-  </si>
-  <si>
-    <t>Concepts in DPV this extends</t>
-  </si>
-  <si>
-    <t>dpv:DataSubjectRight</t>
   </si>
   <si>
     <t>EUFundamentalRights</t>
@@ -409,7 +403,7 @@
     <t>A1 Human Dignity</t>
   </si>
   <si>
-    <t>eu-rights:T1-Dignity,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T1-Dignity</t>
   </si>
   <si>
     <r>
@@ -550,7 +544,7 @@
     <t>A6 Right To Libery Security</t>
   </si>
   <si>
-    <t>eu-rights:T2-Freedoms,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T2-Freedoms</t>
   </si>
   <si>
     <r>
@@ -898,7 +892,7 @@
     <t>A20 Equality Before Law</t>
   </si>
   <si>
-    <t>eu-rights:T3-Equality,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T3-Equality</t>
   </si>
   <si>
     <r>
@@ -1085,7 +1079,7 @@
     <t>A27 Workers Right To Information Consultation</t>
   </si>
   <si>
-    <t>eu-rights:T4-Solidarity,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T4-Solidarity</t>
   </si>
   <si>
     <r>
@@ -1387,7 +1381,7 @@
     <t>A39 Right To Vote Stand As Canditate E U Parliament</t>
   </si>
   <si>
-    <t>eu-rights:T5-CitizensRights,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T5-CitizensRights</t>
   </si>
   <si>
     <r>
@@ -1597,7 +1591,7 @@
     <t>A47 Right To Effective Remedy Fair Trial</t>
   </si>
   <si>
-    <t>eu-rights:T6-Justice,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T6-Justice</t>
   </si>
   <si>
     <r>
@@ -1715,7 +1709,7 @@
     <t>A51 Field Of Application</t>
   </si>
   <si>
-    <t>eu-rights:T7-InterpretationAndApplication,eu-rights:EUFundamentalRights</t>
+    <t>eu-rights:T7-InterpretationAndApplication</t>
   </si>
   <si>
     <r>
@@ -9282,35 +9276,114 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="9" t="s">
+    <row r="3">
+      <c r="A3" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="21">
+        <v>44734.0</v>
+      </c>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="21">
+        <v>44735.0</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>113</v>
+      <c r="A5" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>26</v>
@@ -9320,10 +9393,10 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="40" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="K5" s="21">
-        <v>44734.0</v>
+        <v>44736.0</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="20" t="s">
@@ -9333,7 +9406,7 @@
         <v>75</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
@@ -9352,28 +9425,28 @@
       <c r="AD5" s="19"/>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="41"/>
+      <c r="A6" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="19"/>
       <c r="D6" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="40" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K6" s="21">
-        <v>44735.0</v>
+        <v>44737.0</v>
       </c>
       <c r="L6" s="19"/>
       <c r="M6" s="20" t="s">
@@ -9383,34 +9456,34 @@
         <v>75</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>26</v>
@@ -9420,10 +9493,10 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="40" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="K7" s="21">
-        <v>44736.0</v>
+        <v>44738.0</v>
       </c>
       <c r="L7" s="19"/>
       <c r="M7" s="20" t="s">
@@ -9433,7 +9506,7 @@
         <v>75</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -9453,14 +9526,14 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>26</v>
@@ -9470,10 +9543,10 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="40" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K8" s="21">
-        <v>44737.0</v>
+        <v>44739.0</v>
       </c>
       <c r="L8" s="19"/>
       <c r="M8" s="20" t="s">
@@ -9483,7 +9556,7 @@
         <v>75</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
@@ -9503,14 +9576,14 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>26</v>
@@ -9520,10 +9593,10 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="40" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="K9" s="21">
-        <v>44738.0</v>
+        <v>44740.0</v>
       </c>
       <c r="L9" s="19"/>
       <c r="M9" s="20" t="s">
@@ -9533,7 +9606,7 @@
         <v>75</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
@@ -9552,28 +9625,28 @@
       <c r="AD9" s="19"/>
     </row>
     <row r="10">
-      <c r="A10" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="19"/>
+      <c r="A10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="41"/>
       <c r="D10" s="20" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="40" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="K10" s="21">
-        <v>44739.0</v>
+        <v>44741.0</v>
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="20" t="s">
@@ -9583,34 +9656,34 @@
         <v>75</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>26</v>
@@ -9620,10 +9693,10 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="40" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="K11" s="21">
-        <v>44740.0</v>
+        <v>44742.0</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="20" t="s">
@@ -9633,7 +9706,7 @@
         <v>75</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
@@ -9652,28 +9725,28 @@
       <c r="AD11" s="19"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="41"/>
+      <c r="A12" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="20" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
       <c r="J12" s="40" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K12" s="21">
-        <v>44741.0</v>
+        <v>44743.0</v>
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="20" t="s">
@@ -9683,34 +9756,34 @@
         <v>75</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>26</v>
@@ -9720,10 +9793,10 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="40" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K13" s="21">
-        <v>44742.0</v>
+        <v>44744.0</v>
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="20" t="s">
@@ -9733,7 +9806,7 @@
         <v>75</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
@@ -9753,14 +9826,14 @@
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>26</v>
@@ -9770,10 +9843,10 @@
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="J14" s="40" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="K14" s="21">
-        <v>44743.0</v>
+        <v>44745.0</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="20" t="s">
@@ -9783,7 +9856,7 @@
         <v>75</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
@@ -9803,14 +9876,14 @@
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>26</v>
@@ -9820,10 +9893,10 @@
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="40" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="K15" s="21">
-        <v>44744.0</v>
+        <v>44746.0</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="20" t="s">
@@ -9833,7 +9906,7 @@
         <v>75</v>
       </c>
       <c r="O15" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
@@ -9853,14 +9926,14 @@
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>26</v>
@@ -9870,10 +9943,10 @@
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="40" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="K16" s="21">
-        <v>44745.0</v>
+        <v>44747.0</v>
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="20" t="s">
@@ -9883,7 +9956,7 @@
         <v>75</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
@@ -9903,14 +9976,14 @@
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>26</v>
@@ -9920,10 +9993,10 @@
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="40" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K17" s="21">
-        <v>44746.0</v>
+        <v>44748.0</v>
       </c>
       <c r="L17" s="19"/>
       <c r="M17" s="20" t="s">
@@ -9933,7 +10006,7 @@
         <v>75</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
@@ -9953,14 +10026,14 @@
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>26</v>
@@ -9970,10 +10043,10 @@
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="40" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K18" s="21">
-        <v>44747.0</v>
+        <v>44749.0</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="20" t="s">
@@ -9983,7 +10056,7 @@
         <v>75</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
@@ -10003,14 +10076,14 @@
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>26</v>
@@ -10020,10 +10093,10 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="40" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K19" s="21">
-        <v>44748.0</v>
+        <v>44750.0</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="20" t="s">
@@ -10033,7 +10106,7 @@
         <v>75</v>
       </c>
       <c r="O19" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
@@ -10053,14 +10126,14 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>26</v>
@@ -10070,10 +10143,10 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="40" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K20" s="21">
-        <v>44749.0</v>
+        <v>44751.0</v>
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="20" t="s">
@@ -10083,7 +10156,7 @@
         <v>75</v>
       </c>
       <c r="O20" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
@@ -10103,14 +10176,14 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>26</v>
@@ -10120,10 +10193,10 @@
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="40" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K21" s="21">
-        <v>44750.0</v>
+        <v>44752.0</v>
       </c>
       <c r="L21" s="19"/>
       <c r="M21" s="20" t="s">
@@ -10133,7 +10206,7 @@
         <v>75</v>
       </c>
       <c r="O21" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
@@ -10153,14 +10226,14 @@
     </row>
     <row r="22">
       <c r="A22" s="20" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>26</v>
@@ -10170,10 +10243,10 @@
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="40" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K22" s="21">
-        <v>44751.0</v>
+        <v>44753.0</v>
       </c>
       <c r="L22" s="19"/>
       <c r="M22" s="20" t="s">
@@ -10183,7 +10256,7 @@
         <v>75</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
@@ -10203,14 +10276,14 @@
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>26</v>
@@ -10220,10 +10293,10 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="J23" s="40" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="K23" s="21">
-        <v>44752.0</v>
+        <v>44754.0</v>
       </c>
       <c r="L23" s="19"/>
       <c r="M23" s="20" t="s">
@@ -10233,7 +10306,7 @@
         <v>75</v>
       </c>
       <c r="O23" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
@@ -10253,14 +10326,14 @@
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>26</v>
@@ -10270,10 +10343,10 @@
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="40" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K24" s="21">
-        <v>44753.0</v>
+        <v>44755.0</v>
       </c>
       <c r="L24" s="19"/>
       <c r="M24" s="20" t="s">
@@ -10283,7 +10356,7 @@
         <v>75</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
@@ -10302,28 +10375,28 @@
       <c r="AD24" s="19"/>
     </row>
     <row r="25">
-      <c r="A25" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="C25" s="19"/>
+      <c r="A25" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="41"/>
       <c r="D25" s="20" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
       <c r="J25" s="40" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="K25" s="21">
-        <v>44754.0</v>
+        <v>44756.0</v>
       </c>
       <c r="L25" s="19"/>
       <c r="M25" s="20" t="s">
@@ -10333,34 +10406,34 @@
         <v>75</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="41"/>
+      <c r="AB25" s="41"/>
+      <c r="AC25" s="41"/>
+      <c r="AD25" s="41"/>
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>26</v>
@@ -10370,10 +10443,10 @@
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
       <c r="J26" s="40" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="K26" s="21">
-        <v>44755.0</v>
+        <v>44757.0</v>
       </c>
       <c r="L26" s="19"/>
       <c r="M26" s="20" t="s">
@@ -10383,7 +10456,7 @@
         <v>75</v>
       </c>
       <c r="O26" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
@@ -10402,28 +10475,28 @@
       <c r="AD26" s="19"/>
     </row>
     <row r="27">
-      <c r="A27" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="41"/>
+      <c r="A27" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="19"/>
       <c r="D27" s="20" t="s">
-        <v>118</v>
+        <v>185</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
       <c r="J27" s="40" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="K27" s="21">
-        <v>44756.0</v>
+        <v>44758.0</v>
       </c>
       <c r="L27" s="19"/>
       <c r="M27" s="20" t="s">
@@ -10433,34 +10506,34 @@
         <v>75</v>
       </c>
       <c r="O27" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="41"/>
-      <c r="AC27" s="41"/>
-      <c r="AD27" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>26</v>
@@ -10470,10 +10543,10 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="40" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K28" s="21">
-        <v>44757.0</v>
+        <v>44759.0</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="20" t="s">
@@ -10483,7 +10556,7 @@
         <v>75</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
@@ -10503,14 +10576,14 @@
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>26</v>
@@ -10520,10 +10593,10 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="40" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="K29" s="21">
-        <v>44758.0</v>
+        <v>44760.0</v>
       </c>
       <c r="L29" s="19"/>
       <c r="M29" s="20" t="s">
@@ -10533,7 +10606,7 @@
         <v>75</v>
       </c>
       <c r="O29" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
@@ -10553,14 +10626,14 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C30" s="19"/>
+        <v>197</v>
+      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>26</v>
@@ -10570,10 +10643,10 @@
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="40" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K30" s="21">
-        <v>44759.0</v>
+        <v>44761.0</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="20" t="s">
@@ -10583,7 +10656,7 @@
         <v>75</v>
       </c>
       <c r="O30" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
@@ -10603,14 +10676,14 @@
     </row>
     <row r="31">
       <c r="A31" s="20" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>26</v>
@@ -10620,10 +10693,10 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="40" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K31" s="21">
-        <v>44760.0</v>
+        <v>44762.0</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="20" t="s">
@@ -10633,7 +10706,7 @@
         <v>75</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
@@ -10653,14 +10726,14 @@
     </row>
     <row r="32">
       <c r="A32" s="20" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="C32" s="20"/>
+        <v>203</v>
+      </c>
+      <c r="C32" s="19"/>
       <c r="D32" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>26</v>
@@ -10670,10 +10743,10 @@
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
       <c r="J32" s="40" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K32" s="21">
-        <v>44761.0</v>
+        <v>44763.0</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="20" t="s">
@@ -10683,7 +10756,7 @@
         <v>75</v>
       </c>
       <c r="O32" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P32" s="19"/>
       <c r="Q32" s="19"/>
@@ -10702,28 +10775,28 @@
       <c r="AD32" s="19"/>
     </row>
     <row r="33">
-      <c r="A33" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="C33" s="19"/>
+      <c r="A33" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="41"/>
       <c r="D33" s="20" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
       <c r="J33" s="40" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="K33" s="21">
-        <v>44762.0</v>
+        <v>44764.0</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="20" t="s">
@@ -10733,34 +10806,34 @@
         <v>75</v>
       </c>
       <c r="O33" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="19"/>
-      <c r="Y33" s="19"/>
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="19"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
-      <c r="AD33" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="41"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="41"/>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="41"/>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="41"/>
+      <c r="AD33" s="41"/>
     </row>
     <row r="34">
       <c r="A34" s="20" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="20" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>26</v>
@@ -10770,10 +10843,10 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="40" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K34" s="21">
-        <v>44763.0</v>
+        <v>44765.0</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="20" t="s">
@@ -10783,7 +10856,7 @@
         <v>75</v>
       </c>
       <c r="O34" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
@@ -10802,28 +10875,28 @@
       <c r="AD34" s="19"/>
     </row>
     <row r="35">
-      <c r="A35" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C35" s="41"/>
+      <c r="A35" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="19"/>
       <c r="D35" s="20" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
       <c r="J35" s="40" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="K35" s="21">
-        <v>44764.0</v>
+        <v>44766.0</v>
       </c>
       <c r="L35" s="19"/>
       <c r="M35" s="20" t="s">
@@ -10833,34 +10906,34 @@
         <v>75</v>
       </c>
       <c r="O35" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="41"/>
-      <c r="V35" s="41"/>
-      <c r="W35" s="41"/>
-      <c r="X35" s="41"/>
-      <c r="Y35" s="41"/>
-      <c r="Z35" s="41"/>
-      <c r="AA35" s="41"/>
-      <c r="AB35" s="41"/>
-      <c r="AC35" s="41"/>
-      <c r="AD35" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="19"/>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
     </row>
     <row r="36">
       <c r="A36" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>26</v>
@@ -10870,10 +10943,10 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="40" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K36" s="21">
-        <v>44765.0</v>
+        <v>44767.0</v>
       </c>
       <c r="L36" s="19"/>
       <c r="M36" s="20" t="s">
@@ -10883,7 +10956,7 @@
         <v>75</v>
       </c>
       <c r="O36" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
@@ -10903,14 +10976,14 @@
     </row>
     <row r="37">
       <c r="A37" s="20" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>26</v>
@@ -10920,10 +10993,10 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="40" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K37" s="21">
-        <v>44766.0</v>
+        <v>44768.0</v>
       </c>
       <c r="L37" s="19"/>
       <c r="M37" s="20" t="s">
@@ -10933,7 +11006,7 @@
         <v>75</v>
       </c>
       <c r="O37" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
@@ -10953,14 +11026,14 @@
     </row>
     <row r="38">
       <c r="A38" s="20" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>26</v>
@@ -10970,10 +11043,10 @@
       <c r="H38" s="19"/>
       <c r="I38" s="19"/>
       <c r="J38" s="40" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="K38" s="21">
-        <v>44767.0</v>
+        <v>44769.0</v>
       </c>
       <c r="L38" s="19"/>
       <c r="M38" s="20" t="s">
@@ -10983,7 +11056,7 @@
         <v>75</v>
       </c>
       <c r="O38" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
@@ -11003,14 +11076,14 @@
     </row>
     <row r="39">
       <c r="A39" s="20" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>26</v>
@@ -11020,10 +11093,10 @@
       <c r="H39" s="19"/>
       <c r="I39" s="19"/>
       <c r="J39" s="40" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="K39" s="21">
-        <v>44768.0</v>
+        <v>44770.0</v>
       </c>
       <c r="L39" s="19"/>
       <c r="M39" s="20" t="s">
@@ -11033,7 +11106,7 @@
         <v>75</v>
       </c>
       <c r="O39" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
@@ -11053,14 +11126,14 @@
     </row>
     <row r="40">
       <c r="A40" s="20" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>26</v>
@@ -11070,10 +11143,10 @@
       <c r="H40" s="19"/>
       <c r="I40" s="19"/>
       <c r="J40" s="40" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="K40" s="21">
-        <v>44769.0</v>
+        <v>44771.0</v>
       </c>
       <c r="L40" s="19"/>
       <c r="M40" s="20" t="s">
@@ -11083,7 +11156,7 @@
         <v>75</v>
       </c>
       <c r="O40" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P40" s="19"/>
       <c r="Q40" s="19"/>
@@ -11103,14 +11176,14 @@
     </row>
     <row r="41">
       <c r="A41" s="20" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>26</v>
@@ -11120,10 +11193,10 @@
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
       <c r="J41" s="40" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K41" s="21">
-        <v>44770.0</v>
+        <v>44772.0</v>
       </c>
       <c r="L41" s="19"/>
       <c r="M41" s="20" t="s">
@@ -11133,7 +11206,7 @@
         <v>75</v>
       </c>
       <c r="O41" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -11153,14 +11226,14 @@
     </row>
     <row r="42">
       <c r="A42" s="20" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>26</v>
@@ -11170,10 +11243,10 @@
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
       <c r="J42" s="40" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="K42" s="21">
-        <v>44771.0</v>
+        <v>44773.0</v>
       </c>
       <c r="L42" s="19"/>
       <c r="M42" s="20" t="s">
@@ -11183,7 +11256,7 @@
         <v>75</v>
       </c>
       <c r="O42" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
@@ -11203,14 +11276,14 @@
     </row>
     <row r="43">
       <c r="A43" s="20" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E43" s="20" t="s">
         <v>26</v>
@@ -11220,10 +11293,10 @@
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
       <c r="J43" s="40" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K43" s="21">
-        <v>44772.0</v>
+        <v>44774.0</v>
       </c>
       <c r="L43" s="19"/>
       <c r="M43" s="20" t="s">
@@ -11233,7 +11306,7 @@
         <v>75</v>
       </c>
       <c r="O43" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P43" s="19"/>
       <c r="Q43" s="19"/>
@@ -11253,14 +11326,14 @@
     </row>
     <row r="44">
       <c r="A44" s="20" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>26</v>
@@ -11270,10 +11343,10 @@
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
       <c r="J44" s="40" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K44" s="21">
-        <v>44773.0</v>
+        <v>44775.0</v>
       </c>
       <c r="L44" s="19"/>
       <c r="M44" s="20" t="s">
@@ -11283,7 +11356,7 @@
         <v>75</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P44" s="19"/>
       <c r="Q44" s="19"/>
@@ -11303,14 +11376,14 @@
     </row>
     <row r="45">
       <c r="A45" s="20" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>26</v>
@@ -11320,10 +11393,10 @@
       <c r="H45" s="19"/>
       <c r="I45" s="19"/>
       <c r="J45" s="40" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="K45" s="21">
-        <v>44774.0</v>
+        <v>44776.0</v>
       </c>
       <c r="L45" s="19"/>
       <c r="M45" s="20" t="s">
@@ -11333,7 +11406,7 @@
         <v>75</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P45" s="19"/>
       <c r="Q45" s="19"/>
@@ -11352,28 +11425,28 @@
       <c r="AD45" s="19"/>
     </row>
     <row r="46">
-      <c r="A46" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C46" s="19"/>
+      <c r="A46" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C46" s="41"/>
       <c r="D46" s="20" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
       <c r="J46" s="40" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="K46" s="21">
-        <v>44775.0</v>
+        <v>44777.0</v>
       </c>
       <c r="L46" s="19"/>
       <c r="M46" s="20" t="s">
@@ -11383,34 +11456,34 @@
         <v>75</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
-      <c r="AD46" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="41"/>
+      <c r="R46" s="41"/>
+      <c r="S46" s="41"/>
+      <c r="T46" s="41"/>
+      <c r="U46" s="41"/>
+      <c r="V46" s="41"/>
+      <c r="W46" s="41"/>
+      <c r="X46" s="41"/>
+      <c r="Y46" s="41"/>
+      <c r="Z46" s="41"/>
+      <c r="AA46" s="41"/>
+      <c r="AB46" s="41"/>
+      <c r="AC46" s="41"/>
+      <c r="AD46" s="41"/>
     </row>
     <row r="47">
       <c r="A47" s="20" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="20" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>26</v>
@@ -11420,10 +11493,10 @@
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
       <c r="J47" s="40" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="K47" s="21">
-        <v>44776.0</v>
+        <v>44778.0</v>
       </c>
       <c r="L47" s="19"/>
       <c r="M47" s="20" t="s">
@@ -11433,7 +11506,7 @@
         <v>75</v>
       </c>
       <c r="O47" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P47" s="19"/>
       <c r="Q47" s="19"/>
@@ -11452,28 +11525,28 @@
       <c r="AD47" s="19"/>
     </row>
     <row r="48">
-      <c r="A48" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C48" s="41"/>
+      <c r="A48" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C48" s="19"/>
       <c r="D48" s="20" t="s">
-        <v>118</v>
+        <v>250</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="40" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="K48" s="21">
-        <v>44777.0</v>
+        <v>44779.0</v>
       </c>
       <c r="L48" s="19"/>
       <c r="M48" s="20" t="s">
@@ -11483,34 +11556,34 @@
         <v>75</v>
       </c>
       <c r="O48" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P48" s="41"/>
-      <c r="Q48" s="41"/>
-      <c r="R48" s="41"/>
-      <c r="S48" s="41"/>
-      <c r="T48" s="41"/>
-      <c r="U48" s="41"/>
-      <c r="V48" s="41"/>
-      <c r="W48" s="41"/>
-      <c r="X48" s="41"/>
-      <c r="Y48" s="41"/>
-      <c r="Z48" s="41"/>
-      <c r="AA48" s="41"/>
-      <c r="AB48" s="41"/>
-      <c r="AC48" s="41"/>
-      <c r="AD48" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="19"/>
+      <c r="AB48" s="19"/>
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
     </row>
     <row r="49">
       <c r="A49" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>26</v>
@@ -11520,10 +11593,10 @@
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
       <c r="J49" s="40" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="K49" s="21">
-        <v>44778.0</v>
+        <v>44780.0</v>
       </c>
       <c r="L49" s="19"/>
       <c r="M49" s="20" t="s">
@@ -11533,7 +11606,7 @@
         <v>75</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P49" s="19"/>
       <c r="Q49" s="19"/>
@@ -11553,14 +11626,14 @@
     </row>
     <row r="50">
       <c r="A50" s="20" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>26</v>
@@ -11570,10 +11643,10 @@
       <c r="H50" s="19"/>
       <c r="I50" s="19"/>
       <c r="J50" s="40" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="K50" s="21">
-        <v>44779.0</v>
+        <v>44781.0</v>
       </c>
       <c r="L50" s="19"/>
       <c r="M50" s="20" t="s">
@@ -11583,7 +11656,7 @@
         <v>75</v>
       </c>
       <c r="O50" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P50" s="19"/>
       <c r="Q50" s="19"/>
@@ -11603,14 +11676,14 @@
     </row>
     <row r="51">
       <c r="A51" s="20" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>26</v>
@@ -11620,10 +11693,10 @@
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
       <c r="J51" s="40" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="K51" s="21">
-        <v>44780.0</v>
+        <v>44782.0</v>
       </c>
       <c r="L51" s="19"/>
       <c r="M51" s="20" t="s">
@@ -11633,7 +11706,7 @@
         <v>75</v>
       </c>
       <c r="O51" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
@@ -11653,14 +11726,14 @@
     </row>
     <row r="52">
       <c r="A52" s="20" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>26</v>
@@ -11670,10 +11743,10 @@
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
       <c r="J52" s="40" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="K52" s="21">
-        <v>44781.0</v>
+        <v>44783.0</v>
       </c>
       <c r="L52" s="19"/>
       <c r="M52" s="20" t="s">
@@ -11683,7 +11756,7 @@
         <v>75</v>
       </c>
       <c r="O52" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P52" s="19"/>
       <c r="Q52" s="19"/>
@@ -11703,14 +11776,14 @@
     </row>
     <row r="53">
       <c r="A53" s="20" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>26</v>
@@ -11720,10 +11793,10 @@
       <c r="H53" s="19"/>
       <c r="I53" s="19"/>
       <c r="J53" s="40" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="K53" s="21">
-        <v>44782.0</v>
+        <v>44784.0</v>
       </c>
       <c r="L53" s="19"/>
       <c r="M53" s="20" t="s">
@@ -11733,7 +11806,7 @@
         <v>75</v>
       </c>
       <c r="O53" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P53" s="19"/>
       <c r="Q53" s="19"/>
@@ -11753,14 +11826,14 @@
     </row>
     <row r="54">
       <c r="A54" s="20" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>26</v>
@@ -11770,10 +11843,10 @@
       <c r="H54" s="19"/>
       <c r="I54" s="19"/>
       <c r="J54" s="40" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="K54" s="21">
-        <v>44783.0</v>
+        <v>44785.0</v>
       </c>
       <c r="L54" s="19"/>
       <c r="M54" s="20" t="s">
@@ -11783,7 +11856,7 @@
         <v>75</v>
       </c>
       <c r="O54" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P54" s="19"/>
       <c r="Q54" s="19"/>
@@ -11802,28 +11875,28 @@
       <c r="AD54" s="19"/>
     </row>
     <row r="55">
-      <c r="A55" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C55" s="19"/>
+      <c r="A55" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="B55" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" s="41"/>
       <c r="D55" s="20" t="s">
-        <v>252</v>
+        <v>116</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
       <c r="J55" s="40" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="K55" s="21">
-        <v>44784.0</v>
+        <v>44786.0</v>
       </c>
       <c r="L55" s="19"/>
       <c r="M55" s="20" t="s">
@@ -11833,34 +11906,34 @@
         <v>75</v>
       </c>
       <c r="O55" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="19"/>
-      <c r="R55" s="19"/>
-      <c r="S55" s="19"/>
-      <c r="T55" s="19"/>
-      <c r="U55" s="19"/>
-      <c r="V55" s="19"/>
-      <c r="W55" s="19"/>
-      <c r="X55" s="19"/>
-      <c r="Y55" s="19"/>
-      <c r="Z55" s="19"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="19"/>
-      <c r="AD55" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="P55" s="41"/>
+      <c r="Q55" s="41"/>
+      <c r="R55" s="41"/>
+      <c r="S55" s="41"/>
+      <c r="T55" s="41"/>
+      <c r="U55" s="41"/>
+      <c r="V55" s="41"/>
+      <c r="W55" s="41"/>
+      <c r="X55" s="41"/>
+      <c r="Y55" s="41"/>
+      <c r="Z55" s="41"/>
+      <c r="AA55" s="41"/>
+      <c r="AB55" s="41"/>
+      <c r="AC55" s="41"/>
+      <c r="AD55" s="41"/>
     </row>
     <row r="56">
-      <c r="A56" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>273</v>
+      <c r="A56" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>277</v>
       </c>
       <c r="C56" s="19"/>
-      <c r="D56" s="20" t="s">
-        <v>252</v>
+      <c r="D56" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>26</v>
@@ -11870,10 +11943,10 @@
       <c r="H56" s="19"/>
       <c r="I56" s="19"/>
       <c r="J56" s="40" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="K56" s="21">
-        <v>44785.0</v>
+        <v>44787.0</v>
       </c>
       <c r="L56" s="19"/>
       <c r="M56" s="20" t="s">
@@ -11883,7 +11956,7 @@
         <v>75</v>
       </c>
       <c r="O56" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P56" s="19"/>
       <c r="Q56" s="19"/>
@@ -11902,28 +11975,28 @@
       <c r="AD56" s="19"/>
     </row>
     <row r="57">
-      <c r="A57" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="B57" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="20" t="s">
-        <v>118</v>
+      <c r="A57" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
       <c r="J57" s="40" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K57" s="21">
-        <v>44786.0</v>
+        <v>44788.0</v>
       </c>
       <c r="L57" s="19"/>
       <c r="M57" s="20" t="s">
@@ -11933,34 +12006,34 @@
         <v>75</v>
       </c>
       <c r="O57" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P57" s="41"/>
-      <c r="Q57" s="41"/>
-      <c r="R57" s="41"/>
-      <c r="S57" s="41"/>
-      <c r="T57" s="41"/>
-      <c r="U57" s="41"/>
-      <c r="V57" s="41"/>
-      <c r="W57" s="41"/>
-      <c r="X57" s="41"/>
-      <c r="Y57" s="41"/>
-      <c r="Z57" s="41"/>
-      <c r="AA57" s="41"/>
-      <c r="AB57" s="41"/>
-      <c r="AC57" s="41"/>
-      <c r="AD57" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="19"/>
+      <c r="S57" s="19"/>
+      <c r="T57" s="19"/>
+      <c r="U57" s="19"/>
+      <c r="V57" s="19"/>
+      <c r="W57" s="19"/>
+      <c r="X57" s="19"/>
+      <c r="Y57" s="19"/>
+      <c r="Z57" s="19"/>
+      <c r="AA57" s="19"/>
+      <c r="AB57" s="19"/>
+      <c r="AC57" s="19"/>
+      <c r="AD57" s="19"/>
     </row>
     <row r="58">
       <c r="A58" s="22" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>26</v>
@@ -11970,10 +12043,10 @@
       <c r="H58" s="19"/>
       <c r="I58" s="19"/>
       <c r="J58" s="40" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="K58" s="21">
-        <v>44787.0</v>
+        <v>44789.0</v>
       </c>
       <c r="L58" s="19"/>
       <c r="M58" s="20" t="s">
@@ -11983,7 +12056,7 @@
         <v>75</v>
       </c>
       <c r="O58" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>
@@ -12002,15 +12075,15 @@
       <c r="AD58" s="19"/>
     </row>
     <row r="59">
-      <c r="A59" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>283</v>
+      <c r="A59" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>287</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>26</v>
@@ -12020,10 +12093,10 @@
       <c r="H59" s="19"/>
       <c r="I59" s="19"/>
       <c r="J59" s="40" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="K59" s="21">
-        <v>44788.0</v>
+        <v>44790.0</v>
       </c>
       <c r="L59" s="19"/>
       <c r="M59" s="20" t="s">
@@ -12033,7 +12106,7 @@
         <v>75</v>
       </c>
       <c r="O59" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P59" s="19"/>
       <c r="Q59" s="19"/>
@@ -12052,15 +12125,15 @@
       <c r="AD59" s="19"/>
     </row>
     <row r="60">
-      <c r="A60" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B60" s="22" t="s">
-        <v>286</v>
+      <c r="A60" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="C60" s="19"/>
-      <c r="D60" s="22" t="s">
-        <v>280</v>
+      <c r="D60" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>26</v>
@@ -12070,10 +12143,10 @@
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
       <c r="J60" s="40" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="K60" s="21">
-        <v>44789.0</v>
+        <v>44791.0</v>
       </c>
       <c r="L60" s="19"/>
       <c r="M60" s="20" t="s">
@@ -12083,7 +12156,7 @@
         <v>75</v>
       </c>
       <c r="O60" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P60" s="19"/>
       <c r="Q60" s="19"/>
@@ -12103,14 +12176,14 @@
     </row>
     <row r="61">
       <c r="A61" s="20" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C61" s="19"/>
-      <c r="D61" s="22" t="s">
-        <v>280</v>
+      <c r="D61" s="20" t="s">
+        <v>294</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>26</v>
@@ -12120,10 +12193,10 @@
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
       <c r="J61" s="40" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="K61" s="21">
-        <v>44790.0</v>
+        <v>44792.0</v>
       </c>
       <c r="L61" s="19"/>
       <c r="M61" s="20" t="s">
@@ -12133,7 +12206,7 @@
         <v>75</v>
       </c>
       <c r="O61" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P61" s="19"/>
       <c r="Q61" s="19"/>
@@ -12152,15 +12225,15 @@
       <c r="AD61" s="19"/>
     </row>
     <row r="62">
-      <c r="A62" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>292</v>
+      <c r="A62" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>297</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="20" t="s">
-        <v>118</v>
+        <v>294</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>26</v>
@@ -12170,10 +12243,10 @@
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
       <c r="J62" s="40" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="K62" s="21">
-        <v>44791.0</v>
+        <v>44793.0</v>
       </c>
       <c r="L62" s="19"/>
       <c r="M62" s="20" t="s">
@@ -12183,7 +12256,7 @@
         <v>75</v>
       </c>
       <c r="O62" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P62" s="19"/>
       <c r="Q62" s="19"/>
@@ -12203,14 +12276,14 @@
     </row>
     <row r="63">
       <c r="A63" s="20" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>26</v>
@@ -12220,10 +12293,10 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
       <c r="J63" s="40" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K63" s="21">
-        <v>44792.0</v>
+        <v>44794.0</v>
       </c>
       <c r="L63" s="19"/>
       <c r="M63" s="20" t="s">
@@ -12233,7 +12306,7 @@
         <v>75</v>
       </c>
       <c r="O63" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P63" s="19"/>
       <c r="Q63" s="19"/>
@@ -12253,14 +12326,14 @@
     </row>
     <row r="64">
       <c r="A64" s="20" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>26</v>
@@ -12270,10 +12343,10 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
       <c r="J64" s="40" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="K64" s="21">
-        <v>44793.0</v>
+        <v>44795.0</v>
       </c>
       <c r="L64" s="19"/>
       <c r="M64" s="20" t="s">
@@ -12283,7 +12356,7 @@
         <v>75</v>
       </c>
       <c r="O64" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P64" s="19"/>
       <c r="Q64" s="19"/>
@@ -12302,104 +12375,10 @@
       <c r="AD64" s="19"/>
     </row>
     <row r="65">
-      <c r="A65" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="40" t="s">
-        <v>303</v>
-      </c>
-      <c r="K65" s="21">
-        <v>44794.0</v>
-      </c>
-      <c r="L65" s="19"/>
-      <c r="M65" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="N65" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="O65" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P65" s="19"/>
-      <c r="Q65" s="19"/>
-      <c r="R65" s="19"/>
-      <c r="S65" s="19"/>
-      <c r="T65" s="19"/>
-      <c r="U65" s="19"/>
-      <c r="V65" s="19"/>
-      <c r="W65" s="19"/>
-      <c r="X65" s="19"/>
-      <c r="Y65" s="19"/>
-      <c r="Z65" s="19"/>
-      <c r="AA65" s="19"/>
-      <c r="AB65" s="19"/>
-      <c r="AC65" s="19"/>
-      <c r="AD65" s="19"/>
+      <c r="K65" s="21"/>
     </row>
     <row r="66">
-      <c r="A66" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="B66" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="E66" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="K66" s="21">
-        <v>44795.0</v>
-      </c>
-      <c r="L66" s="19"/>
-      <c r="M66" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="N66" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="O66" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="P66" s="19"/>
-      <c r="Q66" s="19"/>
-      <c r="R66" s="19"/>
-      <c r="S66" s="19"/>
-      <c r="T66" s="19"/>
-      <c r="U66" s="19"/>
-      <c r="V66" s="19"/>
-      <c r="W66" s="19"/>
-      <c r="X66" s="19"/>
-      <c r="Y66" s="19"/>
-      <c r="Z66" s="19"/>
-      <c r="AA66" s="19"/>
-      <c r="AB66" s="19"/>
-      <c r="AC66" s="19"/>
-      <c r="AD66" s="19"/>
+      <c r="K66" s="21"/>
     </row>
     <row r="67">
       <c r="K67" s="21"/>
@@ -12423,52 +12402,60 @@
       <c r="K73" s="21"/>
     </row>
     <row r="74">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="41"/>
       <c r="K74" s="21"/>
+      <c r="L74" s="41"/>
+      <c r="M74" s="9"/>
+      <c r="P74" s="41"/>
+      <c r="Q74" s="41"/>
+      <c r="R74" s="41"/>
+      <c r="S74" s="41"/>
+      <c r="T74" s="41"/>
+      <c r="U74" s="41"/>
+      <c r="V74" s="41"/>
+      <c r="W74" s="41"/>
+      <c r="X74" s="41"/>
+      <c r="Y74" s="41"/>
+      <c r="Z74" s="41"/>
+      <c r="AA74" s="41"/>
+      <c r="AB74" s="41"/>
+      <c r="AC74" s="41"/>
+      <c r="AD74" s="41"/>
     </row>
     <row r="75">
       <c r="K75" s="21"/>
     </row>
     <row r="76">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="41"/>
-      <c r="F76" s="41"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="41"/>
-      <c r="I76" s="41"/>
-      <c r="J76" s="41"/>
       <c r="K76" s="21"/>
-      <c r="L76" s="41"/>
-      <c r="M76" s="9"/>
-      <c r="P76" s="41"/>
-      <c r="Q76" s="41"/>
-      <c r="R76" s="41"/>
-      <c r="S76" s="41"/>
-      <c r="T76" s="41"/>
-      <c r="U76" s="41"/>
-      <c r="V76" s="41"/>
-      <c r="W76" s="41"/>
-      <c r="X76" s="41"/>
-      <c r="Y76" s="41"/>
-      <c r="Z76" s="41"/>
-      <c r="AA76" s="41"/>
-      <c r="AB76" s="41"/>
-      <c r="AC76" s="41"/>
-      <c r="AD76" s="41"/>
     </row>
     <row r="77">
+      <c r="A77" s="42"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="43"/>
       <c r="K77" s="21"/>
     </row>
     <row r="78">
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="45"/>
       <c r="K78" s="21"/>
     </row>
     <row r="79">
-      <c r="A79" s="42"/>
-      <c r="B79" s="42"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="43"/>
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="45"/>
       <c r="K79" s="21"/>
     </row>
     <row r="80">
@@ -12486,9 +12473,9 @@
       <c r="K81" s="21"/>
     </row>
     <row r="82">
-      <c r="A82" s="44"/>
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
+      <c r="A82" s="46"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="46"/>
       <c r="D82" s="45"/>
       <c r="K82" s="21"/>
     </row>
@@ -12496,176 +12483,162 @@
       <c r="A83" s="44"/>
       <c r="B83" s="44"/>
       <c r="C83" s="44"/>
-      <c r="D83" s="45"/>
+      <c r="D83" s="47"/>
       <c r="K83" s="21"/>
     </row>
     <row r="84">
-      <c r="A84" s="46"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="46"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
       <c r="D84" s="45"/>
       <c r="K84" s="21"/>
     </row>
-    <row r="85">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="47"/>
-      <c r="K85" s="21"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="45"/>
-      <c r="K86" s="21"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AD223">
+  <conditionalFormatting sqref="A2:AD221">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB189">
+  <conditionalFormatting sqref="A2:AB187">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C6 D2:D12 E2:E223 F2:I6 J2:O223 P2:AB6 AC2:AD27 A24:C27 D24:D25 F24:I27 P24:AB27 D27:D35 A41:D42 F41:I42 P41:AD42 D48 D57 D62 A66:D223 F66:I223 P66:AD223">
+  <conditionalFormatting sqref="A2:C4 D2:D10 E2:E221 F2:I4 J2:O221 P2:AB4 AC2:AD25 A22:C25 D22:D23 F22:I25 P22:AB25 D25:D33 A39:D40 F39:I40 P39:AD40 D46 D55 D60 A64:D221 F64:I221 P64:AD221">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C6 D2:D12 E2:E223 F2:I6 J2:O223 P2:AB6 AC2:AD27 A24:C27 D24:D25 F24:I27 P24:AB27 D27:D35 A41:D42 F41:I42 P41:AD42 D48 D57 D62 A66:D223 F66:I223 P66:AD223">
+  <conditionalFormatting sqref="A2:C4 D2:D10 E2:E221 F2:I4 J2:O221 P2:AB4 AC2:AD25 A22:C25 D22:D23 F22:I25 P22:AB25 D25:D33 A39:D40 F39:I40 P39:AD40 D46 D55 D60 A64:D221 F64:I221 P64:AD221">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J5"/>
-    <hyperlink r:id="rId2" ref="O5"/>
-    <hyperlink r:id="rId3" ref="J6"/>
-    <hyperlink r:id="rId4" ref="O6"/>
-    <hyperlink r:id="rId5" ref="J7"/>
-    <hyperlink r:id="rId6" ref="O7"/>
-    <hyperlink r:id="rId7" ref="J8"/>
-    <hyperlink r:id="rId8" ref="O8"/>
-    <hyperlink r:id="rId9" ref="J9"/>
-    <hyperlink r:id="rId10" ref="O9"/>
-    <hyperlink r:id="rId11" ref="J10"/>
-    <hyperlink r:id="rId12" ref="O10"/>
-    <hyperlink r:id="rId13" ref="J11"/>
-    <hyperlink r:id="rId14" ref="O11"/>
-    <hyperlink r:id="rId15" ref="J12"/>
-    <hyperlink r:id="rId16" ref="O12"/>
-    <hyperlink r:id="rId17" ref="J13"/>
-    <hyperlink r:id="rId18" ref="O13"/>
-    <hyperlink r:id="rId19" ref="J14"/>
-    <hyperlink r:id="rId20" ref="O14"/>
-    <hyperlink r:id="rId21" ref="J15"/>
-    <hyperlink r:id="rId22" ref="O15"/>
-    <hyperlink r:id="rId23" ref="J16"/>
-    <hyperlink r:id="rId24" ref="O16"/>
-    <hyperlink r:id="rId25" ref="J17"/>
-    <hyperlink r:id="rId26" ref="O17"/>
-    <hyperlink r:id="rId27" ref="J18"/>
-    <hyperlink r:id="rId28" ref="O18"/>
-    <hyperlink r:id="rId29" ref="J19"/>
-    <hyperlink r:id="rId30" ref="O19"/>
-    <hyperlink r:id="rId31" ref="J20"/>
-    <hyperlink r:id="rId32" ref="O20"/>
-    <hyperlink r:id="rId33" ref="J21"/>
-    <hyperlink r:id="rId34" ref="O21"/>
-    <hyperlink r:id="rId35" ref="J22"/>
-    <hyperlink r:id="rId36" ref="O22"/>
-    <hyperlink r:id="rId37" ref="J23"/>
-    <hyperlink r:id="rId38" ref="O23"/>
-    <hyperlink r:id="rId39" ref="J24"/>
-    <hyperlink r:id="rId40" ref="O24"/>
-    <hyperlink r:id="rId41" ref="J25"/>
-    <hyperlink r:id="rId42" ref="O25"/>
-    <hyperlink r:id="rId43" ref="J26"/>
-    <hyperlink r:id="rId44" ref="O26"/>
-    <hyperlink r:id="rId45" ref="J27"/>
-    <hyperlink r:id="rId46" ref="O27"/>
-    <hyperlink r:id="rId47" ref="J28"/>
-    <hyperlink r:id="rId48" ref="O28"/>
-    <hyperlink r:id="rId49" ref="J29"/>
-    <hyperlink r:id="rId50" ref="O29"/>
-    <hyperlink r:id="rId51" ref="J30"/>
-    <hyperlink r:id="rId52" ref="O30"/>
-    <hyperlink r:id="rId53" ref="J31"/>
-    <hyperlink r:id="rId54" ref="O31"/>
-    <hyperlink r:id="rId55" ref="J32"/>
-    <hyperlink r:id="rId56" ref="O32"/>
-    <hyperlink r:id="rId57" ref="J33"/>
-    <hyperlink r:id="rId58" ref="O33"/>
-    <hyperlink r:id="rId59" ref="J34"/>
-    <hyperlink r:id="rId60" ref="O34"/>
-    <hyperlink r:id="rId61" ref="J35"/>
-    <hyperlink r:id="rId62" ref="O35"/>
-    <hyperlink r:id="rId63" ref="J36"/>
-    <hyperlink r:id="rId64" ref="O36"/>
-    <hyperlink r:id="rId65" ref="J37"/>
-    <hyperlink r:id="rId66" ref="O37"/>
-    <hyperlink r:id="rId67" ref="J38"/>
-    <hyperlink r:id="rId68" ref="O38"/>
-    <hyperlink r:id="rId69" ref="J39"/>
-    <hyperlink r:id="rId70" ref="O39"/>
-    <hyperlink r:id="rId71" ref="J40"/>
-    <hyperlink r:id="rId72" ref="O40"/>
-    <hyperlink r:id="rId73" ref="J41"/>
-    <hyperlink r:id="rId74" ref="O41"/>
-    <hyperlink r:id="rId75" ref="J42"/>
-    <hyperlink r:id="rId76" ref="O42"/>
-    <hyperlink r:id="rId77" ref="J43"/>
-    <hyperlink r:id="rId78" ref="O43"/>
-    <hyperlink r:id="rId79" ref="J44"/>
-    <hyperlink r:id="rId80" ref="O44"/>
-    <hyperlink r:id="rId81" ref="J45"/>
-    <hyperlink r:id="rId82" ref="O45"/>
-    <hyperlink r:id="rId83" ref="J46"/>
-    <hyperlink r:id="rId84" ref="O46"/>
-    <hyperlink r:id="rId85" ref="J47"/>
-    <hyperlink r:id="rId86" ref="O47"/>
-    <hyperlink r:id="rId87" ref="J48"/>
-    <hyperlink r:id="rId88" ref="O48"/>
-    <hyperlink r:id="rId89" ref="J49"/>
-    <hyperlink r:id="rId90" ref="O49"/>
-    <hyperlink r:id="rId91" ref="J50"/>
-    <hyperlink r:id="rId92" ref="O50"/>
-    <hyperlink r:id="rId93" ref="J51"/>
-    <hyperlink r:id="rId94" ref="O51"/>
-    <hyperlink r:id="rId95" ref="J52"/>
-    <hyperlink r:id="rId96" ref="O52"/>
-    <hyperlink r:id="rId97" ref="J53"/>
-    <hyperlink r:id="rId98" ref="O53"/>
-    <hyperlink r:id="rId99" ref="J54"/>
-    <hyperlink r:id="rId100" ref="O54"/>
-    <hyperlink r:id="rId101" ref="J55"/>
-    <hyperlink r:id="rId102" ref="O55"/>
-    <hyperlink r:id="rId103" ref="J56"/>
-    <hyperlink r:id="rId104" ref="O56"/>
-    <hyperlink r:id="rId105" ref="J57"/>
-    <hyperlink r:id="rId106" ref="O57"/>
-    <hyperlink r:id="rId107" ref="J58"/>
-    <hyperlink r:id="rId108" ref="O58"/>
-    <hyperlink r:id="rId109" ref="J59"/>
-    <hyperlink r:id="rId110" ref="O59"/>
-    <hyperlink r:id="rId111" ref="J60"/>
-    <hyperlink r:id="rId112" ref="O60"/>
-    <hyperlink r:id="rId113" ref="J61"/>
-    <hyperlink r:id="rId114" ref="O61"/>
-    <hyperlink r:id="rId115" ref="J62"/>
-    <hyperlink r:id="rId116" ref="O62"/>
-    <hyperlink r:id="rId117" ref="J63"/>
-    <hyperlink r:id="rId118" ref="O63"/>
-    <hyperlink r:id="rId119" ref="J64"/>
-    <hyperlink r:id="rId120" ref="O64"/>
-    <hyperlink r:id="rId121" ref="J65"/>
-    <hyperlink r:id="rId122" ref="O65"/>
-    <hyperlink r:id="rId123" ref="J66"/>
-    <hyperlink r:id="rId124" ref="O66"/>
+    <hyperlink r:id="rId1" ref="J3"/>
+    <hyperlink r:id="rId2" ref="O3"/>
+    <hyperlink r:id="rId3" ref="J4"/>
+    <hyperlink r:id="rId4" ref="O4"/>
+    <hyperlink r:id="rId5" ref="J5"/>
+    <hyperlink r:id="rId6" ref="O5"/>
+    <hyperlink r:id="rId7" ref="J6"/>
+    <hyperlink r:id="rId8" ref="O6"/>
+    <hyperlink r:id="rId9" ref="J7"/>
+    <hyperlink r:id="rId10" ref="O7"/>
+    <hyperlink r:id="rId11" ref="J8"/>
+    <hyperlink r:id="rId12" ref="O8"/>
+    <hyperlink r:id="rId13" ref="J9"/>
+    <hyperlink r:id="rId14" ref="O9"/>
+    <hyperlink r:id="rId15" ref="J10"/>
+    <hyperlink r:id="rId16" ref="O10"/>
+    <hyperlink r:id="rId17" ref="J11"/>
+    <hyperlink r:id="rId18" ref="O11"/>
+    <hyperlink r:id="rId19" ref="J12"/>
+    <hyperlink r:id="rId20" ref="O12"/>
+    <hyperlink r:id="rId21" ref="J13"/>
+    <hyperlink r:id="rId22" ref="O13"/>
+    <hyperlink r:id="rId23" ref="J14"/>
+    <hyperlink r:id="rId24" ref="O14"/>
+    <hyperlink r:id="rId25" ref="J15"/>
+    <hyperlink r:id="rId26" ref="O15"/>
+    <hyperlink r:id="rId27" ref="J16"/>
+    <hyperlink r:id="rId28" ref="O16"/>
+    <hyperlink r:id="rId29" ref="J17"/>
+    <hyperlink r:id="rId30" ref="O17"/>
+    <hyperlink r:id="rId31" ref="J18"/>
+    <hyperlink r:id="rId32" ref="O18"/>
+    <hyperlink r:id="rId33" ref="J19"/>
+    <hyperlink r:id="rId34" ref="O19"/>
+    <hyperlink r:id="rId35" ref="J20"/>
+    <hyperlink r:id="rId36" ref="O20"/>
+    <hyperlink r:id="rId37" ref="J21"/>
+    <hyperlink r:id="rId38" ref="O21"/>
+    <hyperlink r:id="rId39" ref="J22"/>
+    <hyperlink r:id="rId40" ref="O22"/>
+    <hyperlink r:id="rId41" ref="J23"/>
+    <hyperlink r:id="rId42" ref="O23"/>
+    <hyperlink r:id="rId43" ref="J24"/>
+    <hyperlink r:id="rId44" ref="O24"/>
+    <hyperlink r:id="rId45" ref="J25"/>
+    <hyperlink r:id="rId46" ref="O25"/>
+    <hyperlink r:id="rId47" ref="J26"/>
+    <hyperlink r:id="rId48" ref="O26"/>
+    <hyperlink r:id="rId49" ref="J27"/>
+    <hyperlink r:id="rId50" ref="O27"/>
+    <hyperlink r:id="rId51" ref="J28"/>
+    <hyperlink r:id="rId52" ref="O28"/>
+    <hyperlink r:id="rId53" ref="J29"/>
+    <hyperlink r:id="rId54" ref="O29"/>
+    <hyperlink r:id="rId55" ref="J30"/>
+    <hyperlink r:id="rId56" ref="O30"/>
+    <hyperlink r:id="rId57" ref="J31"/>
+    <hyperlink r:id="rId58" ref="O31"/>
+    <hyperlink r:id="rId59" ref="J32"/>
+    <hyperlink r:id="rId60" ref="O32"/>
+    <hyperlink r:id="rId61" ref="J33"/>
+    <hyperlink r:id="rId62" ref="O33"/>
+    <hyperlink r:id="rId63" ref="J34"/>
+    <hyperlink r:id="rId64" ref="O34"/>
+    <hyperlink r:id="rId65" ref="J35"/>
+    <hyperlink r:id="rId66" ref="O35"/>
+    <hyperlink r:id="rId67" ref="J36"/>
+    <hyperlink r:id="rId68" ref="O36"/>
+    <hyperlink r:id="rId69" ref="J37"/>
+    <hyperlink r:id="rId70" ref="O37"/>
+    <hyperlink r:id="rId71" ref="J38"/>
+    <hyperlink r:id="rId72" ref="O38"/>
+    <hyperlink r:id="rId73" ref="J39"/>
+    <hyperlink r:id="rId74" ref="O39"/>
+    <hyperlink r:id="rId75" ref="J40"/>
+    <hyperlink r:id="rId76" ref="O40"/>
+    <hyperlink r:id="rId77" ref="J41"/>
+    <hyperlink r:id="rId78" ref="O41"/>
+    <hyperlink r:id="rId79" ref="J42"/>
+    <hyperlink r:id="rId80" ref="O42"/>
+    <hyperlink r:id="rId81" ref="J43"/>
+    <hyperlink r:id="rId82" ref="O43"/>
+    <hyperlink r:id="rId83" ref="J44"/>
+    <hyperlink r:id="rId84" ref="O44"/>
+    <hyperlink r:id="rId85" ref="J45"/>
+    <hyperlink r:id="rId86" ref="O45"/>
+    <hyperlink r:id="rId87" ref="J46"/>
+    <hyperlink r:id="rId88" ref="O46"/>
+    <hyperlink r:id="rId89" ref="J47"/>
+    <hyperlink r:id="rId90" ref="O47"/>
+    <hyperlink r:id="rId91" ref="J48"/>
+    <hyperlink r:id="rId92" ref="O48"/>
+    <hyperlink r:id="rId93" ref="J49"/>
+    <hyperlink r:id="rId94" ref="O49"/>
+    <hyperlink r:id="rId95" ref="J50"/>
+    <hyperlink r:id="rId96" ref="O50"/>
+    <hyperlink r:id="rId97" ref="J51"/>
+    <hyperlink r:id="rId98" ref="O51"/>
+    <hyperlink r:id="rId99" ref="J52"/>
+    <hyperlink r:id="rId100" ref="O52"/>
+    <hyperlink r:id="rId101" ref="J53"/>
+    <hyperlink r:id="rId102" ref="O53"/>
+    <hyperlink r:id="rId103" ref="J54"/>
+    <hyperlink r:id="rId104" ref="O54"/>
+    <hyperlink r:id="rId105" ref="J55"/>
+    <hyperlink r:id="rId106" ref="O55"/>
+    <hyperlink r:id="rId107" ref="J56"/>
+    <hyperlink r:id="rId108" ref="O56"/>
+    <hyperlink r:id="rId109" ref="J57"/>
+    <hyperlink r:id="rId110" ref="O57"/>
+    <hyperlink r:id="rId111" ref="J58"/>
+    <hyperlink r:id="rId112" ref="O58"/>
+    <hyperlink r:id="rId113" ref="J59"/>
+    <hyperlink r:id="rId114" ref="O59"/>
+    <hyperlink r:id="rId115" ref="J60"/>
+    <hyperlink r:id="rId116" ref="O60"/>
+    <hyperlink r:id="rId117" ref="J61"/>
+    <hyperlink r:id="rId118" ref="O61"/>
+    <hyperlink r:id="rId119" ref="J62"/>
+    <hyperlink r:id="rId120" ref="O62"/>
+    <hyperlink r:id="rId121" ref="J63"/>
+    <hyperlink r:id="rId122" ref="O63"/>
+    <hyperlink r:id="rId123" ref="J64"/>
+    <hyperlink r:id="rId124" ref="O64"/>
   </hyperlinks>
   <drawing r:id="rId125"/>
 </worksheet>

</xml_diff>

<commit_message>
adds documentation for rights module in DPV
- adds documentation for rights module in DPV
- adds examples
- changes intro in rules DPV module HTML
- adds explanation for types of rules in rules DPV module HTML
- adds concept RightNotice to rights module in DPV as a parent of
  RightExerciseNotice, and makes RightExerciseNotice the parent of
  RightFulfilmentNotice and RightNonFulfilmentNotice
- in rights properties in DPV, moves 'definition' from reused concept to
  be 'usage notes' instead so as to avoid multiple definitions
</commit_message>
<xml_diff>
--- a/code/vocab_csv/rights.xlsx
+++ b/code/vocab_csv/rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="310">
   <si>
     <t>Term</t>
   </si>
@@ -135,16 +135,37 @@
     <t>Exercising Rights</t>
   </si>
   <si>
+    <t>RightNotice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Notice </t>
+  </si>
+  <si>
+    <t>Information associated with rights, such as which rights exist, when and where they are applicable, and other relevant information</t>
+  </si>
+  <si>
+    <t>dpv:Notice</t>
+  </si>
+  <si>
+    <t>dpv:OrganisationalMeasure</t>
+  </si>
+  <si>
+    <t>This concept also covers information about rights exercise, with dpv:RightExerciseNotice specifically representing information provided in connection with exercising of rights. Both notices may be needed, e.g. RightNotice for providing information about existence and exercise of rights, and RightExerciseNotice for providing additional information specifically about exericse of rights - such as to request more information or provide updates on an exercised rights request</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit</t>
+  </si>
+  <si>
     <t>RightExerciseNotice</t>
   </si>
   <si>
     <t>Right Exercise Notice</t>
   </si>
   <si>
-    <t>Information associated with exercising of an active right</t>
-  </si>
-  <si>
-    <t>dpv:OrganisationalMeasure</t>
+    <t>Information associated with exercising of an active right such as where and how to exercise the right, information required for it, or updates on an exercised rights request</t>
+  </si>
+  <si>
+    <t>dpv:RightNotice</t>
   </si>
   <si>
     <t>This concept is intended for providing information regarding a right exercise. For specific instances of such exercises, see RightExerciseActivity and RightExerciseRecord.</t>
@@ -192,7 +213,7 @@
     <t>Notice provided regarding fulfilment of a right</t>
   </si>
   <si>
-    <t>dpv:Notice</t>
+    <t>dpv:RightExerciseNotice</t>
   </si>
   <si>
     <t>This notice is associated with situations where information is provided with the intention of progressing the fulfilment of a right. For example, a notice asking for more information regarding the scope of the right, or providing information on where to access the data provided under a right.</t>
@@ -240,9 +261,6 @@
     <t>dpv:Relation</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit</t>
-  </si>
-  <si>
     <t>isExercisedAt</t>
   </si>
   <si>
@@ -255,39 +273,36 @@
     <t>dpv:ActiveRight</t>
   </si>
   <si>
-    <t>dpv:RightExerciseNotice</t>
-  </si>
-  <si>
     <t>dpv:hasStatus</t>
   </si>
   <si>
+    <t>dpv:RightExerciseActivity</t>
+  </si>
+  <si>
+    <t>dpv:Status</t>
+  </si>
+  <si>
     <t>Indicates the status of a Right Exercise Activity</t>
   </si>
   <si>
-    <t>dpv:RightExerciseActivity</t>
-  </si>
-  <si>
-    <t>dpv:Status</t>
-  </si>
-  <si>
     <t>dpv:hasRecipient</t>
   </si>
   <si>
+    <t>dpv:Recipient</t>
+  </si>
+  <si>
     <t>Indicates the Recipient of a Right Exercise Activity</t>
   </si>
   <si>
-    <t>dpv:Recipient</t>
-  </si>
-  <si>
     <t>dpv:isImplementedByEntity</t>
   </si>
   <si>
+    <t>dpv:Entity</t>
+  </si>
+  <si>
     <t>Indicates the Entity that implements or performs a Right Exercise Activity</t>
   </si>
   <si>
-    <t>dpv:Entity</t>
-  </si>
-  <si>
     <t>foaf:page</t>
   </si>
   <si>
@@ -297,12 +312,12 @@
     <t>dct:hasPart</t>
   </si>
   <si>
+    <t>dpv:RightExerciseRecord</t>
+  </si>
+  <si>
     <t>Specifying a RightExerciseRecord has RightExerciseActivity as part of its records</t>
   </si>
   <si>
-    <t>dpv:RightExerciseRecord</t>
-  </si>
-  <si>
     <t>dct:isPartOf</t>
   </si>
   <si>
@@ -321,10 +336,10 @@
     <t>dpv:hasJustification</t>
   </si>
   <si>
+    <t>dpv:Justification</t>
+  </si>
+  <si>
     <t>Specifying a justification for non-fulfilment of Right Exercise</t>
-  </si>
-  <si>
-    <t>dpv:Justification</t>
   </si>
   <si>
     <t>dct:format</t>
@@ -2699,30 +2714,30 @@
       <c r="C10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="E10" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10" s="23"/>
       <c r="K10" s="21">
-        <v>44856.0</v>
+        <v>45459.0</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="24" t="s">
-        <v>45</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="O10" s="20"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
       <c r="R10" s="19"/>
@@ -2739,29 +2754,31 @@
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="J11" s="23"/>
       <c r="K11" s="21">
-        <v>44867.0</v>
-      </c>
-      <c r="L11" s="19"/>
+        <v>44856.0</v>
+      </c>
+      <c r="L11" s="21"/>
       <c r="M11" s="20" t="s">
         <v>20</v>
       </c>
@@ -2769,7 +2786,7 @@
         <v>34</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
@@ -2787,25 +2804,23 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>53</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D12" s="19"/>
       <c r="E12" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="21">
@@ -2819,7 +2834,7 @@
         <v>34</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
@@ -2836,96 +2851,96 @@
       <c r="AB12" s="19"/>
     </row>
     <row r="13">
-      <c r="B13" s="22"/>
-      <c r="C13" s="25"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="O13" s="27"/>
+      <c r="A13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="21">
+        <v>44867.0</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="B14" s="22"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="C14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="O14" s="27"/>
     </row>
     <row r="15">
-      <c r="A15" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="21">
-        <v>44867.0</v>
-      </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
+      <c r="A15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="21">
@@ -2935,11 +2950,11 @@
       <c r="M16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="28" t="s">
-        <v>61</v>
+      <c r="N16" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
@@ -2956,55 +2971,102 @@
       <c r="AB16" s="19"/>
     </row>
     <row r="17">
-      <c r="A17" s="20"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="19"/>
+      <c r="K17" s="21">
+        <v>44867.0</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
     </row>
     <row r="18">
-      <c r="A18" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="20" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="29"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="21">
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="21">
         <v>44867.0</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20" t="s">
+      <c r="L19" s="19"/>
+      <c r="M19" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="29"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
     </row>
     <row r="20">
       <c r="B20" s="29"/>
@@ -5562,34 +5624,37 @@
     <row r="871">
       <c r="B871" s="29"/>
     </row>
+    <row r="872">
+      <c r="B872" s="29"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AF2 N4:N12">
+  <conditionalFormatting sqref="A2:AF2 N4:N13">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF2 N4:N12">
+  <conditionalFormatting sqref="A2:AF2 N4:N13">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB200">
+  <conditionalFormatting sqref="A2:AB201">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB17 AC2:AF821 A19:AB821">
+  <conditionalFormatting sqref="A2:AB18 AC2:AF822 A20:AB822">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="O2"/>
-    <hyperlink r:id="rId2" ref="O10"/>
-    <hyperlink r:id="rId3" ref="O11"/>
-    <hyperlink r:id="rId4" ref="O12"/>
-    <hyperlink r:id="rId5" ref="O15"/>
-    <hyperlink r:id="rId6" ref="O16"/>
+    <hyperlink r:id="rId2" ref="O11"/>
+    <hyperlink r:id="rId3" ref="O12"/>
+    <hyperlink r:id="rId4" ref="O13"/>
+    <hyperlink r:id="rId5" ref="O16"/>
+    <hyperlink r:id="rId6" ref="O17"/>
   </hyperlinks>
   <drawing r:id="rId7"/>
 </worksheet>
@@ -5629,13 +5694,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -5667,13 +5732,13 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>17</v>
@@ -5682,7 +5747,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -5696,7 +5761,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O2" s="33" t="s">
         <v>22</v>
@@ -5717,22 +5782,22 @@
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -5746,7 +5811,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="18" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O3" s="33" t="s">
         <v>22</v>
@@ -5767,26 +5832,26 @@
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="I4" s="25" t="s">
+        <v>89</v>
+      </c>
       <c r="J4" s="19"/>
       <c r="K4" s="21"/>
       <c r="L4" s="19"/>
@@ -5813,26 +5878,26 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>86</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="I5" s="25" t="s">
+        <v>92</v>
+      </c>
       <c r="J5" s="19"/>
       <c r="K5" s="21"/>
       <c r="L5" s="19"/>
@@ -5859,26 +5924,26 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>89</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C6" s="19"/>
       <c r="D6" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="J6" s="19"/>
       <c r="K6" s="21"/>
       <c r="L6" s="19"/>
@@ -5905,24 +5970,24 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>92</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="25" t="s">
+        <v>97</v>
+      </c>
       <c r="J7" s="19"/>
       <c r="K7" s="21"/>
       <c r="L7" s="19"/>
@@ -5949,26 +6014,26 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>94</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C8" s="19"/>
       <c r="D8" s="20" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="25" t="s">
+        <v>100</v>
+      </c>
       <c r="J8" s="19"/>
       <c r="K8" s="21"/>
       <c r="L8" s="19"/>
@@ -5995,26 +6060,26 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>97</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="25" t="s">
+        <v>102</v>
+      </c>
       <c r="J9" s="19"/>
       <c r="K9" s="21"/>
       <c r="L9" s="19"/>
@@ -6041,26 +6106,26 @@
     </row>
     <row r="10">
       <c r="A10" s="20" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>99</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="I10" s="25" t="s">
+        <v>104</v>
+      </c>
       <c r="J10" s="19"/>
       <c r="K10" s="21"/>
       <c r="L10" s="19"/>
@@ -6087,26 +6152,26 @@
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>99</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C11" s="19"/>
       <c r="D11" s="34" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="34" t="s">
+        <v>104</v>
+      </c>
       <c r="J11" s="19"/>
       <c r="K11" s="21"/>
       <c r="L11" s="19"/>
@@ -6133,26 +6198,26 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>102</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="25" t="s">
+        <v>108</v>
+      </c>
       <c r="J12" s="19"/>
       <c r="K12" s="21"/>
       <c r="L12" s="19"/>
@@ -6179,22 +6244,22 @@
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>105</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="20" t="s">
+        <v>110</v>
+      </c>
       <c r="J13" s="19"/>
       <c r="K13" s="21"/>
       <c r="L13" s="19"/>
@@ -6221,22 +6286,22 @@
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>107</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="J14" s="19"/>
       <c r="K14" s="21"/>
       <c r="L14" s="19"/>
@@ -6263,22 +6328,22 @@
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>109</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="25" t="s">
+        <v>114</v>
+      </c>
       <c r="J15" s="19"/>
       <c r="K15" s="21"/>
       <c r="L15" s="19"/>
@@ -9278,10 +9343,10 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -9293,7 +9358,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="40" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K3" s="21">
         <v>44734.0</v>
@@ -9303,10 +9368,10 @@
         <v>20</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
@@ -9326,14 +9391,14 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>26</v>
@@ -9343,7 +9408,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="41"/>
       <c r="J4" s="40" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="K4" s="21">
         <v>44735.0</v>
@@ -9353,10 +9418,10 @@
         <v>20</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
@@ -9376,14 +9441,14 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>26</v>
@@ -9393,7 +9458,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="40" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="K5" s="21">
         <v>44736.0</v>
@@ -9403,10 +9468,10 @@
         <v>20</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
@@ -9426,14 +9491,14 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>26</v>
@@ -9443,7 +9508,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="40" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="K6" s="21">
         <v>44737.0</v>
@@ -9453,10 +9518,10 @@
         <v>20</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
@@ -9476,14 +9541,14 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>26</v>
@@ -9493,7 +9558,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="40" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K7" s="21">
         <v>44738.0</v>
@@ -9503,10 +9568,10 @@
         <v>20</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -9526,14 +9591,14 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>26</v>
@@ -9543,7 +9608,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="40" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="K8" s="21">
         <v>44739.0</v>
@@ -9553,10 +9618,10 @@
         <v>20</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
@@ -9576,14 +9641,14 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>26</v>
@@ -9593,7 +9658,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="40" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="K9" s="21">
         <v>44740.0</v>
@@ -9603,10 +9668,10 @@
         <v>20</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
@@ -9626,14 +9691,14 @@
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>26</v>
@@ -9643,7 +9708,7 @@
       <c r="H10" s="41"/>
       <c r="I10" s="41"/>
       <c r="J10" s="40" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="K10" s="21">
         <v>44741.0</v>
@@ -9653,10 +9718,10 @@
         <v>20</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
@@ -9676,14 +9741,14 @@
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>26</v>
@@ -9693,7 +9758,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="40" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="K11" s="21">
         <v>44742.0</v>
@@ -9703,10 +9768,10 @@
         <v>20</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
@@ -9726,14 +9791,14 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>26</v>
@@ -9743,7 +9808,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="40" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="K12" s="21">
         <v>44743.0</v>
@@ -9753,10 +9818,10 @@
         <v>20</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
@@ -9776,14 +9841,14 @@
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>26</v>
@@ -9793,7 +9858,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="40" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="K13" s="21">
         <v>44744.0</v>
@@ -9803,10 +9868,10 @@
         <v>20</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
@@ -9826,14 +9891,14 @@
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>26</v>
@@ -9843,7 +9908,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="J14" s="40" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="K14" s="21">
         <v>44745.0</v>
@@ -9853,10 +9918,10 @@
         <v>20</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
@@ -9876,14 +9941,14 @@
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>26</v>
@@ -9893,7 +9958,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="40" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="K15" s="21">
         <v>44746.0</v>
@@ -9903,10 +9968,10 @@
         <v>20</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O15" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
@@ -9926,14 +9991,14 @@
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>26</v>
@@ -9943,7 +10008,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="40" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K16" s="21">
         <v>44747.0</v>
@@ -9953,10 +10018,10 @@
         <v>20</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
@@ -9976,14 +10041,14 @@
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>26</v>
@@ -9993,7 +10058,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="40" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="K17" s="21">
         <v>44748.0</v>
@@ -10003,10 +10068,10 @@
         <v>20</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
@@ -10026,14 +10091,14 @@
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>26</v>
@@ -10043,7 +10108,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="40" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K18" s="21">
         <v>44749.0</v>
@@ -10053,10 +10118,10 @@
         <v>20</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
@@ -10076,14 +10141,14 @@
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>26</v>
@@ -10093,7 +10158,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="40" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="K19" s="21">
         <v>44750.0</v>
@@ -10103,10 +10168,10 @@
         <v>20</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O19" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
@@ -10126,14 +10191,14 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>26</v>
@@ -10143,7 +10208,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="40" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="K20" s="21">
         <v>44751.0</v>
@@ -10153,10 +10218,10 @@
         <v>20</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O20" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
@@ -10176,14 +10241,14 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>26</v>
@@ -10193,7 +10258,7 @@
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="40" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K21" s="21">
         <v>44752.0</v>
@@ -10203,10 +10268,10 @@
         <v>20</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O21" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
@@ -10226,14 +10291,14 @@
     </row>
     <row r="22">
       <c r="A22" s="20" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>26</v>
@@ -10243,7 +10308,7 @@
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="40" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="K22" s="21">
         <v>44753.0</v>
@@ -10253,10 +10318,10 @@
         <v>20</v>
       </c>
       <c r="N22" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
@@ -10276,14 +10341,14 @@
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>26</v>
@@ -10293,7 +10358,7 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="J23" s="40" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="K23" s="21">
         <v>44754.0</v>
@@ -10303,10 +10368,10 @@
         <v>20</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O23" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
@@ -10326,14 +10391,14 @@
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>26</v>
@@ -10343,7 +10408,7 @@
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="40" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K24" s="21">
         <v>44755.0</v>
@@ -10353,10 +10418,10 @@
         <v>20</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
@@ -10376,14 +10441,14 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>26</v>
@@ -10393,7 +10458,7 @@
       <c r="H25" s="41"/>
       <c r="I25" s="41"/>
       <c r="J25" s="40" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="K25" s="21">
         <v>44756.0</v>
@@ -10403,10 +10468,10 @@
         <v>20</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P25" s="41"/>
       <c r="Q25" s="41"/>
@@ -10426,14 +10491,14 @@
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>26</v>
@@ -10443,7 +10508,7 @@
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
       <c r="J26" s="40" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="K26" s="21">
         <v>44757.0</v>
@@ -10453,10 +10518,10 @@
         <v>20</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O26" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
@@ -10476,14 +10541,14 @@
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>26</v>
@@ -10493,7 +10558,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="40" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="K27" s="21">
         <v>44758.0</v>
@@ -10503,10 +10568,10 @@
         <v>20</v>
       </c>
       <c r="N27" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O27" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
@@ -10526,14 +10591,14 @@
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>26</v>
@@ -10543,7 +10608,7 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="40" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="K28" s="21">
         <v>44759.0</v>
@@ -10553,10 +10618,10 @@
         <v>20</v>
       </c>
       <c r="N28" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
@@ -10576,14 +10641,14 @@
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>26</v>
@@ -10593,7 +10658,7 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="40" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="K29" s="21">
         <v>44760.0</v>
@@ -10603,10 +10668,10 @@
         <v>20</v>
       </c>
       <c r="N29" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O29" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
@@ -10626,14 +10691,14 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>26</v>
@@ -10643,7 +10708,7 @@
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="40" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="K30" s="21">
         <v>44761.0</v>
@@ -10653,10 +10718,10 @@
         <v>20</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O30" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
@@ -10676,14 +10741,14 @@
     </row>
     <row r="31">
       <c r="A31" s="20" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>26</v>
@@ -10693,7 +10758,7 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="40" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="K31" s="21">
         <v>44762.0</v>
@@ -10703,10 +10768,10 @@
         <v>20</v>
       </c>
       <c r="N31" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
@@ -10726,14 +10791,14 @@
     </row>
     <row r="32">
       <c r="A32" s="20" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="20" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>26</v>
@@ -10743,7 +10808,7 @@
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
       <c r="J32" s="40" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="K32" s="21">
         <v>44763.0</v>
@@ -10753,10 +10818,10 @@
         <v>20</v>
       </c>
       <c r="N32" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O32" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P32" s="19"/>
       <c r="Q32" s="19"/>
@@ -10776,14 +10841,14 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C33" s="41"/>
       <c r="D33" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>26</v>
@@ -10793,7 +10858,7 @@
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
       <c r="J33" s="40" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="K33" s="21">
         <v>44764.0</v>
@@ -10803,10 +10868,10 @@
         <v>20</v>
       </c>
       <c r="N33" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O33" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P33" s="41"/>
       <c r="Q33" s="41"/>
@@ -10826,14 +10891,14 @@
     </row>
     <row r="34">
       <c r="A34" s="20" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>26</v>
@@ -10843,7 +10908,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="40" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="K34" s="21">
         <v>44765.0</v>
@@ -10853,10 +10918,10 @@
         <v>20</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O34" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
@@ -10876,14 +10941,14 @@
     </row>
     <row r="35">
       <c r="A35" s="20" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>26</v>
@@ -10893,7 +10958,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="40" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="K35" s="21">
         <v>44766.0</v>
@@ -10903,10 +10968,10 @@
         <v>20</v>
       </c>
       <c r="N35" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O35" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
@@ -10926,14 +10991,14 @@
     </row>
     <row r="36">
       <c r="A36" s="20" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>26</v>
@@ -10943,7 +11008,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="40" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="K36" s="21">
         <v>44767.0</v>
@@ -10953,10 +11018,10 @@
         <v>20</v>
       </c>
       <c r="N36" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O36" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
@@ -10976,14 +11041,14 @@
     </row>
     <row r="37">
       <c r="A37" s="20" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>26</v>
@@ -10993,7 +11058,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="40" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="K37" s="21">
         <v>44768.0</v>
@@ -11003,10 +11068,10 @@
         <v>20</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O37" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
@@ -11026,14 +11091,14 @@
     </row>
     <row r="38">
       <c r="A38" s="20" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>26</v>
@@ -11043,7 +11108,7 @@
       <c r="H38" s="19"/>
       <c r="I38" s="19"/>
       <c r="J38" s="40" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K38" s="21">
         <v>44769.0</v>
@@ -11053,10 +11118,10 @@
         <v>20</v>
       </c>
       <c r="N38" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O38" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
@@ -11076,14 +11141,14 @@
     </row>
     <row r="39">
       <c r="A39" s="20" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>26</v>
@@ -11093,7 +11158,7 @@
       <c r="H39" s="19"/>
       <c r="I39" s="19"/>
       <c r="J39" s="40" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="K39" s="21">
         <v>44770.0</v>
@@ -11103,10 +11168,10 @@
         <v>20</v>
       </c>
       <c r="N39" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O39" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
@@ -11126,14 +11191,14 @@
     </row>
     <row r="40">
       <c r="A40" s="20" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>26</v>
@@ -11143,7 +11208,7 @@
       <c r="H40" s="19"/>
       <c r="I40" s="19"/>
       <c r="J40" s="40" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="K40" s="21">
         <v>44771.0</v>
@@ -11153,10 +11218,10 @@
         <v>20</v>
       </c>
       <c r="N40" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O40" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P40" s="19"/>
       <c r="Q40" s="19"/>
@@ -11176,14 +11241,14 @@
     </row>
     <row r="41">
       <c r="A41" s="20" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>26</v>
@@ -11193,7 +11258,7 @@
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
       <c r="J41" s="40" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="K41" s="21">
         <v>44772.0</v>
@@ -11203,10 +11268,10 @@
         <v>20</v>
       </c>
       <c r="N41" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O41" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -11226,14 +11291,14 @@
     </row>
     <row r="42">
       <c r="A42" s="20" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>26</v>
@@ -11243,7 +11308,7 @@
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
       <c r="J42" s="40" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="K42" s="21">
         <v>44773.0</v>
@@ -11253,10 +11318,10 @@
         <v>20</v>
       </c>
       <c r="N42" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O42" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
@@ -11276,14 +11341,14 @@
     </row>
     <row r="43">
       <c r="A43" s="20" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E43" s="20" t="s">
         <v>26</v>
@@ -11293,7 +11358,7 @@
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
       <c r="J43" s="40" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="K43" s="21">
         <v>44774.0</v>
@@ -11303,10 +11368,10 @@
         <v>20</v>
       </c>
       <c r="N43" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O43" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P43" s="19"/>
       <c r="Q43" s="19"/>
@@ -11326,14 +11391,14 @@
     </row>
     <row r="44">
       <c r="A44" s="20" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>26</v>
@@ -11343,7 +11408,7 @@
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
       <c r="J44" s="40" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="K44" s="21">
         <v>44775.0</v>
@@ -11353,10 +11418,10 @@
         <v>20</v>
       </c>
       <c r="N44" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P44" s="19"/>
       <c r="Q44" s="19"/>
@@ -11376,14 +11441,14 @@
     </row>
     <row r="45">
       <c r="A45" s="20" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="20" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>26</v>
@@ -11393,7 +11458,7 @@
       <c r="H45" s="19"/>
       <c r="I45" s="19"/>
       <c r="J45" s="40" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="K45" s="21">
         <v>44776.0</v>
@@ -11403,10 +11468,10 @@
         <v>20</v>
       </c>
       <c r="N45" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P45" s="19"/>
       <c r="Q45" s="19"/>
@@ -11426,14 +11491,14 @@
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C46" s="41"/>
       <c r="D46" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>26</v>
@@ -11443,7 +11508,7 @@
       <c r="H46" s="41"/>
       <c r="I46" s="41"/>
       <c r="J46" s="40" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="K46" s="21">
         <v>44777.0</v>
@@ -11453,10 +11518,10 @@
         <v>20</v>
       </c>
       <c r="N46" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P46" s="41"/>
       <c r="Q46" s="41"/>
@@ -11476,14 +11541,14 @@
     </row>
     <row r="47">
       <c r="A47" s="20" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>26</v>
@@ -11493,7 +11558,7 @@
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
       <c r="J47" s="40" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="K47" s="21">
         <v>44778.0</v>
@@ -11503,10 +11568,10 @@
         <v>20</v>
       </c>
       <c r="N47" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O47" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P47" s="19"/>
       <c r="Q47" s="19"/>
@@ -11526,14 +11591,14 @@
     </row>
     <row r="48">
       <c r="A48" s="20" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>26</v>
@@ -11543,7 +11608,7 @@
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
       <c r="J48" s="40" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="K48" s="21">
         <v>44779.0</v>
@@ -11553,10 +11618,10 @@
         <v>20</v>
       </c>
       <c r="N48" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O48" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P48" s="19"/>
       <c r="Q48" s="19"/>
@@ -11576,14 +11641,14 @@
     </row>
     <row r="49">
       <c r="A49" s="20" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>26</v>
@@ -11593,7 +11658,7 @@
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
       <c r="J49" s="40" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="K49" s="21">
         <v>44780.0</v>
@@ -11603,10 +11668,10 @@
         <v>20</v>
       </c>
       <c r="N49" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P49" s="19"/>
       <c r="Q49" s="19"/>
@@ -11626,14 +11691,14 @@
     </row>
     <row r="50">
       <c r="A50" s="20" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>26</v>
@@ -11643,7 +11708,7 @@
       <c r="H50" s="19"/>
       <c r="I50" s="19"/>
       <c r="J50" s="40" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="K50" s="21">
         <v>44781.0</v>
@@ -11653,10 +11718,10 @@
         <v>20</v>
       </c>
       <c r="N50" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O50" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P50" s="19"/>
       <c r="Q50" s="19"/>
@@ -11676,14 +11741,14 @@
     </row>
     <row r="51">
       <c r="A51" s="20" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>26</v>
@@ -11693,7 +11758,7 @@
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
       <c r="J51" s="40" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="K51" s="21">
         <v>44782.0</v>
@@ -11703,10 +11768,10 @@
         <v>20</v>
       </c>
       <c r="N51" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O51" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
@@ -11726,14 +11791,14 @@
     </row>
     <row r="52">
       <c r="A52" s="20" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>26</v>
@@ -11743,7 +11808,7 @@
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
       <c r="J52" s="40" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="K52" s="21">
         <v>44783.0</v>
@@ -11753,10 +11818,10 @@
         <v>20</v>
       </c>
       <c r="N52" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O52" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P52" s="19"/>
       <c r="Q52" s="19"/>
@@ -11776,14 +11841,14 @@
     </row>
     <row r="53">
       <c r="A53" s="20" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>26</v>
@@ -11793,7 +11858,7 @@
       <c r="H53" s="19"/>
       <c r="I53" s="19"/>
       <c r="J53" s="40" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="K53" s="21">
         <v>44784.0</v>
@@ -11803,10 +11868,10 @@
         <v>20</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O53" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P53" s="19"/>
       <c r="Q53" s="19"/>
@@ -11826,14 +11891,14 @@
     </row>
     <row r="54">
       <c r="A54" s="20" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>26</v>
@@ -11843,7 +11908,7 @@
       <c r="H54" s="19"/>
       <c r="I54" s="19"/>
       <c r="J54" s="40" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="K54" s="21">
         <v>44785.0</v>
@@ -11853,10 +11918,10 @@
         <v>20</v>
       </c>
       <c r="N54" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O54" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P54" s="19"/>
       <c r="Q54" s="19"/>
@@ -11876,14 +11941,14 @@
     </row>
     <row r="55">
       <c r="A55" s="42" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C55" s="41"/>
       <c r="D55" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>26</v>
@@ -11893,7 +11958,7 @@
       <c r="H55" s="41"/>
       <c r="I55" s="41"/>
       <c r="J55" s="40" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="K55" s="21">
         <v>44786.0</v>
@@ -11903,10 +11968,10 @@
         <v>20</v>
       </c>
       <c r="N55" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O55" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P55" s="41"/>
       <c r="Q55" s="41"/>
@@ -11926,14 +11991,14 @@
     </row>
     <row r="56">
       <c r="A56" s="22" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="22" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>26</v>
@@ -11943,7 +12008,7 @@
       <c r="H56" s="19"/>
       <c r="I56" s="19"/>
       <c r="J56" s="40" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="K56" s="21">
         <v>44787.0</v>
@@ -11953,10 +12018,10 @@
         <v>20</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O56" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P56" s="19"/>
       <c r="Q56" s="19"/>
@@ -11976,14 +12041,14 @@
     </row>
     <row r="57">
       <c r="A57" s="22" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="22" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>26</v>
@@ -11993,7 +12058,7 @@
       <c r="H57" s="19"/>
       <c r="I57" s="19"/>
       <c r="J57" s="40" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="K57" s="21">
         <v>44788.0</v>
@@ -12003,10 +12068,10 @@
         <v>20</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O57" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P57" s="19"/>
       <c r="Q57" s="19"/>
@@ -12026,14 +12091,14 @@
     </row>
     <row r="58">
       <c r="A58" s="22" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="22" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>26</v>
@@ -12043,7 +12108,7 @@
       <c r="H58" s="19"/>
       <c r="I58" s="19"/>
       <c r="J58" s="40" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="K58" s="21">
         <v>44789.0</v>
@@ -12053,10 +12118,10 @@
         <v>20</v>
       </c>
       <c r="N58" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O58" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>
@@ -12076,14 +12141,14 @@
     </row>
     <row r="59">
       <c r="A59" s="20" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="22" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>26</v>
@@ -12093,7 +12158,7 @@
       <c r="H59" s="19"/>
       <c r="I59" s="19"/>
       <c r="J59" s="40" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="K59" s="21">
         <v>44790.0</v>
@@ -12103,10 +12168,10 @@
         <v>20</v>
       </c>
       <c r="N59" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O59" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P59" s="19"/>
       <c r="Q59" s="19"/>
@@ -12126,14 +12191,14 @@
     </row>
     <row r="60">
       <c r="A60" s="9" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>26</v>
@@ -12143,7 +12208,7 @@
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
       <c r="J60" s="40" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="K60" s="21">
         <v>44791.0</v>
@@ -12153,10 +12218,10 @@
         <v>20</v>
       </c>
       <c r="N60" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O60" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P60" s="19"/>
       <c r="Q60" s="19"/>
@@ -12176,14 +12241,14 @@
     </row>
     <row r="61">
       <c r="A61" s="20" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="20" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>26</v>
@@ -12193,7 +12258,7 @@
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
       <c r="J61" s="40" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="K61" s="21">
         <v>44792.0</v>
@@ -12203,10 +12268,10 @@
         <v>20</v>
       </c>
       <c r="N61" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O61" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P61" s="19"/>
       <c r="Q61" s="19"/>
@@ -12226,14 +12291,14 @@
     </row>
     <row r="62">
       <c r="A62" s="20" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="20" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>26</v>
@@ -12243,7 +12308,7 @@
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
       <c r="J62" s="40" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="K62" s="21">
         <v>44793.0</v>
@@ -12253,10 +12318,10 @@
         <v>20</v>
       </c>
       <c r="N62" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O62" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P62" s="19"/>
       <c r="Q62" s="19"/>
@@ -12276,14 +12341,14 @@
     </row>
     <row r="63">
       <c r="A63" s="20" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="20" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>26</v>
@@ -12293,7 +12358,7 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
       <c r="J63" s="40" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="K63" s="21">
         <v>44794.0</v>
@@ -12303,10 +12368,10 @@
         <v>20</v>
       </c>
       <c r="N63" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O63" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P63" s="19"/>
       <c r="Q63" s="19"/>
@@ -12326,14 +12391,14 @@
     </row>
     <row r="64">
       <c r="A64" s="20" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="20" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>26</v>
@@ -12343,7 +12408,7 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
       <c r="J64" s="40" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="K64" s="21">
         <v>44795.0</v>
@@ -12353,10 +12418,10 @@
         <v>20</v>
       </c>
       <c r="N64" s="20" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O64" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P64" s="19"/>
       <c r="Q64" s="19"/>

</xml_diff>

<commit_message>
updates DPV, TECH, RISK, EU GDPR, AIAct, RIGHTS
- DPV: updates HTML with issues
- TECH: fixes provision method concepts, updates HTML
- RISK: updates HTML
- GDPR: updates rights impacts concepts, updates HTML
- AIAct: updates sectors, updates HTML
- EU Rights: updates granular impacts, updates HTML
</commit_message>
<xml_diff>
--- a/code/vocab_csv/rights.xlsx
+++ b/code/vocab_csv/rights.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="624">
   <si>
     <t>Term</t>
   </si>
@@ -3472,6 +3472,9 @@
   </si>
   <si>
     <t>eu-rights:A8-ProtectionOfPersonalDataImpact</t>
+  </si>
+  <si>
+    <t>This concept is experimental and may change in future versions</t>
   </si>
   <si>
     <r>
@@ -18342,9 +18345,11 @@
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
+      <c r="J66" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K66" s="40" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="L66" s="21">
         <v>45587.0</v>
@@ -18373,13 +18378,13 @@
     </row>
     <row r="67">
       <c r="A67" s="10" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D67" s="20" t="s">
         <v>573</v>
@@ -18393,9 +18398,11 @@
       </c>
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
+      <c r="J67" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K67" s="40" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="L67" s="21">
         <v>45587.0</v>
@@ -18424,13 +18431,13 @@
     </row>
     <row r="68">
       <c r="A68" s="10" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D68" s="20" t="s">
         <v>573</v>
@@ -18444,9 +18451,11 @@
       </c>
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
+      <c r="J68" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K68" s="40" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="L68" s="21">
         <v>45587.0</v>
@@ -18475,13 +18484,13 @@
     </row>
     <row r="69">
       <c r="A69" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>573</v>
@@ -18495,9 +18504,11 @@
       </c>
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
+      <c r="J69" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K69" s="40" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="L69" s="21">
         <v>45587.0</v>
@@ -18526,13 +18537,13 @@
     </row>
     <row r="70">
       <c r="A70" s="10" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D70" s="20" t="s">
         <v>573</v>
@@ -18546,9 +18557,11 @@
       </c>
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
+      <c r="J70" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K70" s="40" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="L70" s="21">
         <v>45587.0</v>
@@ -18577,13 +18590,13 @@
     </row>
     <row r="71">
       <c r="A71" s="10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>573</v>
@@ -18597,9 +18610,11 @@
       </c>
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
-      <c r="J71" s="19"/>
+      <c r="J71" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K71" s="40" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L71" s="21">
         <v>45587.0</v>
@@ -18628,13 +18643,13 @@
     </row>
     <row r="72">
       <c r="A72" s="10" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>573</v>
@@ -18648,9 +18663,11 @@
       </c>
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
+      <c r="J72" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K72" s="40" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="L72" s="21">
         <v>45587.0</v>
@@ -18686,7 +18703,6 @@
       <c r="G73" s="41"/>
       <c r="H73" s="41"/>
       <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
       <c r="K73" s="41"/>
       <c r="L73" s="21"/>
       <c r="M73" s="41"/>
@@ -18709,13 +18725,13 @@
     </row>
     <row r="74">
       <c r="A74" s="20" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>573</v>
@@ -18729,9 +18745,11 @@
       </c>
       <c r="H74" s="19"/>
       <c r="I74" s="19"/>
-      <c r="J74" s="19"/>
+      <c r="J74" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K74" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="L74" s="21">
         <v>45587.0</v>
@@ -18760,13 +18778,13 @@
     </row>
     <row r="75">
       <c r="A75" s="20" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>573</v>
@@ -18780,9 +18798,11 @@
       </c>
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
-      <c r="J75" s="19"/>
+      <c r="J75" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K75" s="40" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="L75" s="21">
         <v>45587.0</v>
@@ -18811,13 +18831,13 @@
     </row>
     <row r="76">
       <c r="A76" s="22" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>573</v>
@@ -18831,9 +18851,11 @@
       </c>
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
+      <c r="J76" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K76" s="40" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="L76" s="21">
         <v>45587.0</v>
@@ -18862,13 +18884,13 @@
     </row>
     <row r="77">
       <c r="A77" s="46" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B77" s="46" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C77" s="46" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>573</v>
@@ -18882,9 +18904,11 @@
       </c>
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
+      <c r="J77" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K77" s="40" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="L77" s="21">
         <v>45587.0</v>
@@ -18913,13 +18937,13 @@
     </row>
     <row r="78">
       <c r="A78" s="46" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C78" s="46" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>573</v>
@@ -18933,9 +18957,11 @@
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
-      <c r="J78" s="19"/>
+      <c r="J78" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K78" s="40" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="L78" s="21">
         <v>45587.0</v>
@@ -18964,13 +18990,13 @@
     </row>
     <row r="79">
       <c r="A79" s="46" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B79" s="46" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C79" s="46" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>573</v>
@@ -18984,9 +19010,11 @@
       </c>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
+      <c r="J79" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="K79" s="40" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="L79" s="21">
         <v>45587.0</v>

</xml_diff>